<commit_message>
refactor: add an explanation to the classic 26th task
</commit_message>
<xml_diff>
--- a/Bariants/kompege-25003936/task_26_1.xlsx
+++ b/Bariants/kompege-25003936/task_26_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htmlprogrammist/Python/ege/Bariants/kompege-25003936/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0E5FA8-19FC-4C4E-BC76-D8D902ECBA43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE0331B-3E91-3C49-ACB6-65ACCA23F42E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="460" windowWidth="28100" windowHeight="16100" xr2:uid="{48522007-5C25-CA43-9FED-8C8FDDDACD5B}"/>
   </bookViews>
@@ -25,9 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>delta</t>
+  </si>
+  <si>
+    <t>Надо было определить минимальное количество контейнеров, которое невозможно перевезти за один раз</t>
+  </si>
+  <si>
+    <t>Т.е. надо как можно больше маленьких перевозить, чтобы как можно больше контейнеров увезти</t>
+  </si>
+  <si>
+    <t>Поэтому сортируем по возрастанию</t>
+  </si>
+  <si>
+    <t>И при этом мы получаем наибольшую возможную суммарную массу, а это то, что нам надо было найти</t>
   </si>
 </sst>
 </file>
@@ -400,7 +412,7 @@
   <dimension ref="A1:E9864"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2195" workbookViewId="0">
-      <selection activeCell="C2208" sqref="C2208"/>
+      <selection activeCell="E2214" sqref="E2214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -20321,13 +20333,16 @@
         <v>100074</v>
       </c>
       <c r="C2211" s="1">
-        <f>9864-2209</f>
+        <f>COUNT(A2210:A10000)</f>
         <v>7655</v>
       </c>
       <c r="D2211" s="1">
         <f>SUM(A2210:A10000)</f>
         <v>542450</v>
       </c>
+      <c r="E2211" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2212" spans="1:5">
       <c r="A2212">
@@ -20337,6 +20352,9 @@
         <f t="shared" si="34"/>
         <v>100125</v>
       </c>
+      <c r="E2212" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2213" spans="1:5">
       <c r="A2213">
@@ -20346,6 +20364,9 @@
         <f t="shared" si="34"/>
         <v>100176</v>
       </c>
+      <c r="E2213" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2214" spans="1:5">
       <c r="A2214">
@@ -20354,6 +20375,9 @@
       <c r="B2214">
         <f t="shared" si="34"/>
         <v>100227</v>
+      </c>
+      <c r="E2214" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2215" spans="1:5">

</xml_diff>

<commit_message>
fix: add python solution to 26th task from variant and add some description to excel's solution
</commit_message>
<xml_diff>
--- a/Bariants/kompege-25003936/task_26_1.xlsx
+++ b/Bariants/kompege-25003936/task_26_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htmlprogrammist/Python/ege/Bariants/kompege-25003936/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE0331B-3E91-3C49-ACB6-65ACCA23F42E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511EC180-CA3F-934B-A807-CE515CBAD29D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="460" windowWidth="28100" windowHeight="16100" xr2:uid="{48522007-5C25-CA43-9FED-8C8FDDDACD5B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>delta</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>И при этом мы получаем наибольшую возможную суммарную массу, а это то, что нам надо было найти</t>
+  </si>
+  <si>
+    <t>Мы не выбрасываем последний груз, чтобы полностью забить корабль контейнерами, потому что: количество-то ладно, оно не изменится, но вот…</t>
+  </si>
+  <si>
+    <t>… наибольшая возможная суммарная масса станет меньше, а это не по условию задачи. Поэтому мы ничего не заменяем, а тупо считаем</t>
   </si>
 </sst>
 </file>
@@ -409,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8CC9267-0E56-9644-803A-0C5CD3830057}">
-  <dimension ref="A1:E9864"/>
+  <dimension ref="A1:F9864"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2195" workbookViewId="0">
-      <selection activeCell="E2214" sqref="E2214"/>
+    <sheetView tabSelected="1" topLeftCell="A2203" workbookViewId="0">
+      <selection activeCell="F2210" sqref="F2210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -20298,7 +20304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2209" spans="1:5">
+    <row r="2209" spans="1:6">
       <c r="A2209">
         <v>51</v>
       </c>
@@ -20314,8 +20320,11 @@
         <f>15 + 51</f>
         <v>66</v>
       </c>
-    </row>
-    <row r="2210" spans="1:5">
+      <c r="F2209" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2210" spans="1:6">
       <c r="A2210">
         <v>51</v>
       </c>
@@ -20323,8 +20332,11 @@
         <f t="shared" si="34"/>
         <v>100023</v>
       </c>
-    </row>
-    <row r="2211" spans="1:5">
+      <c r="F2210" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2211" spans="1:6">
       <c r="A2211">
         <v>51</v>
       </c>
@@ -20344,7 +20356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2212" spans="1:5">
+    <row r="2212" spans="1:6">
       <c r="A2212">
         <v>51</v>
       </c>
@@ -20356,7 +20368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2213" spans="1:5">
+    <row r="2213" spans="1:6">
       <c r="A2213">
         <v>51</v>
       </c>
@@ -20368,7 +20380,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2214" spans="1:5">
+    <row r="2214" spans="1:6">
       <c r="A2214">
         <v>51</v>
       </c>
@@ -20380,7 +20392,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2215" spans="1:5">
+    <row r="2215" spans="1:6">
       <c r="A2215">
         <v>51</v>
       </c>
@@ -20389,7 +20401,7 @@
         <v>100278</v>
       </c>
     </row>
-    <row r="2216" spans="1:5">
+    <row r="2216" spans="1:6">
       <c r="A2216">
         <v>51</v>
       </c>
@@ -20398,7 +20410,7 @@
         <v>100329</v>
       </c>
     </row>
-    <row r="2217" spans="1:5">
+    <row r="2217" spans="1:6">
       <c r="A2217">
         <v>51</v>
       </c>
@@ -20407,7 +20419,7 @@
         <v>100380</v>
       </c>
     </row>
-    <row r="2218" spans="1:5">
+    <row r="2218" spans="1:6">
       <c r="A2218">
         <v>51</v>
       </c>
@@ -20416,7 +20428,7 @@
         <v>100431</v>
       </c>
     </row>
-    <row r="2219" spans="1:5">
+    <row r="2219" spans="1:6">
       <c r="A2219">
         <v>51</v>
       </c>
@@ -20425,7 +20437,7 @@
         <v>100482</v>
       </c>
     </row>
-    <row r="2220" spans="1:5">
+    <row r="2220" spans="1:6">
       <c r="A2220">
         <v>51</v>
       </c>
@@ -20434,7 +20446,7 @@
         <v>100533</v>
       </c>
     </row>
-    <row r="2221" spans="1:5">
+    <row r="2221" spans="1:6">
       <c r="A2221">
         <v>51</v>
       </c>
@@ -20443,7 +20455,7 @@
         <v>100584</v>
       </c>
     </row>
-    <row r="2222" spans="1:5">
+    <row r="2222" spans="1:6">
       <c r="A2222">
         <v>51</v>
       </c>
@@ -20452,7 +20464,7 @@
         <v>100635</v>
       </c>
     </row>
-    <row r="2223" spans="1:5">
+    <row r="2223" spans="1:6">
       <c r="A2223">
         <v>51</v>
       </c>
@@ -20461,7 +20473,7 @@
         <v>100686</v>
       </c>
     </row>
-    <row r="2224" spans="1:5">
+    <row r="2224" spans="1:6">
       <c r="A2224">
         <v>51</v>
       </c>

</xml_diff>